<commit_message>
finished 2nd experiment result
</commit_message>
<xml_diff>
--- a/report/fig_calculated_needed_torque.xlsx
+++ b/report/fig_calculated_needed_torque.xlsx
@@ -2850,7 +2850,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="2005150351"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="-1.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
@@ -3896,7 +3896,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X4" sqref="X4:X202"/>
+      <selection pane="bottomRight" activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>